<commit_message>
Updated data and tasks
</commit_message>
<xml_diff>
--- a/data/Survey Data.xlsx
+++ b/data/Survey Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tonym\Documents\GitHub\example-project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3DFD28-0911-4DF6-9E92-0E67890A4331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EC8877-61FC-4836-BC77-667409CF68EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5528E795-C791-435E-807B-E00EFF8F35A1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5528E795-C791-435E-807B-E00EFF8F35A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="236">
   <si>
     <t>Name</t>
   </si>
@@ -636,6 +636,114 @@
   </si>
   <si>
     <t>Aiden</t>
+  </si>
+  <si>
+    <t>Esther</t>
+  </si>
+  <si>
+    <t>Nala</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>Phillip</t>
+  </si>
+  <si>
+    <t>Yuri</t>
+  </si>
+  <si>
+    <t>Ernest</t>
+  </si>
+  <si>
+    <t>Ivy</t>
+  </si>
+  <si>
+    <t>Jonas</t>
+  </si>
+  <si>
+    <t>Jason</t>
+  </si>
+  <si>
+    <t>Phil</t>
+  </si>
+  <si>
+    <t>Kendrick</t>
+  </si>
+  <si>
+    <t>Farah</t>
+  </si>
+  <si>
+    <t>Lucy</t>
+  </si>
+  <si>
+    <t>Lori</t>
+  </si>
+  <si>
+    <t>Scott</t>
+  </si>
+  <si>
+    <t>Waldo</t>
+  </si>
+  <si>
+    <t>Tomas</t>
+  </si>
+  <si>
+    <t>Miles</t>
+  </si>
+  <si>
+    <t>Hope</t>
+  </si>
+  <si>
+    <t>Ethan</t>
+  </si>
+  <si>
+    <t>Abraham</t>
+  </si>
+  <si>
+    <t>Joshua</t>
+  </si>
+  <si>
+    <t>Abel</t>
+  </si>
+  <si>
+    <t>Muhammad</t>
+  </si>
+  <si>
+    <t>Maged</t>
+  </si>
+  <si>
+    <t>Cage</t>
+  </si>
+  <si>
+    <t>Chase</t>
+  </si>
+  <si>
+    <t>Victor</t>
+  </si>
+  <si>
+    <t>Victoria</t>
+  </si>
+  <si>
+    <t>Terrance</t>
+  </si>
+  <si>
+    <t>Terri</t>
+  </si>
+  <si>
+    <t>Beth</t>
+  </si>
+  <si>
+    <t>Ellen</t>
+  </si>
+  <si>
+    <t>Elvis</t>
   </si>
 </sst>
 </file>
@@ -1007,16 +1115,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAFBF133-D857-474C-9FAB-94F41B7F049F}">
-  <dimension ref="A1:K187"/>
+  <dimension ref="A1:K223"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A188" sqref="A188"/>
+      <pane ySplit="1" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A224" sqref="A224"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1051,7 +1159,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1086,7 +1194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1118,7 +1226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1144,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1170,7 +1278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1199,7 +1307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1228,7 +1336,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1257,7 +1365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1286,7 +1394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1312,7 +1420,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1341,7 +1449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1370,7 +1478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1396,7 +1504,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1422,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1454,7 +1562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1480,7 +1588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1509,7 +1617,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1535,7 +1643,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1564,7 +1672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1596,7 +1704,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1625,7 +1733,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1651,7 +1759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1677,7 +1785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1706,7 +1814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1732,7 +1840,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1761,7 +1869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1787,7 +1895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1813,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1842,7 +1950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -1868,7 +1976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1897,7 +2005,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -1926,7 +2034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -1952,7 +2060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -1978,7 +2086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -2007,7 +2115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -2032,8 +2140,11 @@
       <c r="I36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -2059,7 +2170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -2091,7 +2202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -2120,7 +2231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -2146,7 +2257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -2175,7 +2286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -2207,7 +2318,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -2233,7 +2344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -2262,7 +2373,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -2288,7 +2399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -2317,7 +2428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -2343,7 +2454,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -2372,7 +2483,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -2401,7 +2512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -2427,7 +2538,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -2456,7 +2567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>57</v>
       </c>
@@ -2482,7 +2593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -2508,7 +2619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>59</v>
       </c>
@@ -2537,7 +2648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -2569,7 +2680,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -2598,7 +2709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>62</v>
       </c>
@@ -2630,7 +2741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -2659,7 +2770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>64</v>
       </c>
@@ -2688,7 +2799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>65</v>
       </c>
@@ -2714,7 +2825,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>66</v>
       </c>
@@ -2740,7 +2851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>67</v>
       </c>
@@ -2766,7 +2877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>68</v>
       </c>
@@ -2792,7 +2903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -2818,7 +2929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -2844,7 +2955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -2870,7 +2981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>73</v>
       </c>
@@ -2902,7 +3013,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -2931,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -2957,7 +3068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -2983,7 +3094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -3009,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -3035,7 +3146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -3061,7 +3172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -3087,7 +3198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -3113,7 +3224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -3139,7 +3250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -3168,7 +3279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -3197,7 +3308,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>85</v>
       </c>
@@ -3223,7 +3334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>86</v>
       </c>
@@ -3249,7 +3360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>87</v>
       </c>
@@ -3275,7 +3386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -3304,7 +3415,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -3333,7 +3444,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -3359,7 +3470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -3385,7 +3496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>92</v>
       </c>
@@ -3411,7 +3522,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>93</v>
       </c>
@@ -3437,7 +3548,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>94</v>
       </c>
@@ -3463,7 +3574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>95</v>
       </c>
@@ -3489,7 +3600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>96</v>
       </c>
@@ -3515,7 +3626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>97</v>
       </c>
@@ -3541,7 +3652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>98</v>
       </c>
@@ -3567,7 +3678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>99</v>
       </c>
@@ -3593,7 +3704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>100</v>
       </c>
@@ -3622,7 +3733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>101</v>
       </c>
@@ -3648,7 +3759,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>102</v>
       </c>
@@ -3677,7 +3788,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>103</v>
       </c>
@@ -3703,7 +3814,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>104</v>
       </c>
@@ -3729,7 +3840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>105</v>
       </c>
@@ -3755,7 +3866,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>106</v>
       </c>
@@ -3781,7 +3892,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>107</v>
       </c>
@@ -3807,7 +3918,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>111</v>
       </c>
@@ -3833,7 +3944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>112</v>
       </c>
@@ -3859,7 +3970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>113</v>
       </c>
@@ -3885,7 +3996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>116</v>
       </c>
@@ -3914,7 +4025,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>117</v>
       </c>
@@ -3940,7 +4051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>118</v>
       </c>
@@ -3966,7 +4077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>119</v>
       </c>
@@ -3992,7 +4103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>120</v>
       </c>
@@ -4018,7 +4129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>121</v>
       </c>
@@ -4047,7 +4158,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>122</v>
       </c>
@@ -4076,7 +4187,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>123</v>
       </c>
@@ -4102,7 +4213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>124</v>
       </c>
@@ -4131,7 +4242,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>125</v>
       </c>
@@ -4163,7 +4274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>126</v>
       </c>
@@ -4189,7 +4300,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>127</v>
       </c>
@@ -4215,7 +4326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>128</v>
       </c>
@@ -4241,7 +4352,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>129</v>
       </c>
@@ -4267,7 +4378,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>130</v>
       </c>
@@ -4293,7 +4404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>131</v>
       </c>
@@ -4319,7 +4430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>132</v>
       </c>
@@ -4344,8 +4455,11 @@
       <c r="I121">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>133</v>
       </c>
@@ -4371,7 +4485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>134</v>
       </c>
@@ -4397,7 +4511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>135</v>
       </c>
@@ -4423,7 +4537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>136</v>
       </c>
@@ -4449,7 +4563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>137</v>
       </c>
@@ -4475,7 +4589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>138</v>
       </c>
@@ -4501,7 +4615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>139</v>
       </c>
@@ -4527,7 +4641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>140</v>
       </c>
@@ -4553,7 +4667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>141</v>
       </c>
@@ -4579,7 +4693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>142</v>
       </c>
@@ -4605,7 +4719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>143</v>
       </c>
@@ -4631,7 +4745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>144</v>
       </c>
@@ -4656,8 +4770,11 @@
       <c r="I133">
         <v>1</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>145</v>
       </c>
@@ -4686,7 +4803,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>146</v>
       </c>
@@ -4712,7 +4829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>147</v>
       </c>
@@ -4738,7 +4855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>148</v>
       </c>
@@ -4764,7 +4881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>149</v>
       </c>
@@ -4790,7 +4907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>150</v>
       </c>
@@ -4816,7 +4933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>151</v>
       </c>
@@ -4842,7 +4959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>152</v>
       </c>
@@ -4868,7 +4985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>153</v>
       </c>
@@ -4894,7 +5011,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>154</v>
       </c>
@@ -4920,7 +5037,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>155</v>
       </c>
@@ -4946,7 +5063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>156</v>
       </c>
@@ -4972,7 +5089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>157</v>
       </c>
@@ -4998,7 +5115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>158</v>
       </c>
@@ -5024,7 +5141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>159</v>
       </c>
@@ -5050,7 +5167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>160</v>
       </c>
@@ -5076,7 +5193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>161</v>
       </c>
@@ -5105,7 +5222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>162</v>
       </c>
@@ -5131,7 +5248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>163</v>
       </c>
@@ -5157,7 +5274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>164</v>
       </c>
@@ -5183,7 +5300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>165</v>
       </c>
@@ -5212,7 +5329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>166</v>
       </c>
@@ -5241,7 +5358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>167</v>
       </c>
@@ -5270,7 +5387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>168</v>
       </c>
@@ -5296,7 +5413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>169</v>
       </c>
@@ -5322,7 +5439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>170</v>
       </c>
@@ -5348,7 +5465,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>171</v>
       </c>
@@ -5374,7 +5491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>172</v>
       </c>
@@ -5400,7 +5517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>173</v>
       </c>
@@ -5426,7 +5543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>174</v>
       </c>
@@ -5455,7 +5572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>175</v>
       </c>
@@ -5481,7 +5598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>176</v>
       </c>
@@ -5507,7 +5624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>177</v>
       </c>
@@ -5536,7 +5653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>178</v>
       </c>
@@ -5562,7 +5679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>179</v>
       </c>
@@ -5591,7 +5708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>180</v>
       </c>
@@ -5617,7 +5734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>181</v>
       </c>
@@ -5643,7 +5760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>182</v>
       </c>
@@ -5669,7 +5786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>183</v>
       </c>
@@ -5695,7 +5812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>184</v>
       </c>
@@ -5721,7 +5838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>185</v>
       </c>
@@ -5747,7 +5864,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>186</v>
       </c>
@@ -5773,7 +5890,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>187</v>
       </c>
@@ -5802,7 +5919,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>188</v>
       </c>
@@ -5828,7 +5945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>189</v>
       </c>
@@ -5857,7 +5974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>190</v>
       </c>
@@ -5883,7 +6000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>191</v>
       </c>
@@ -5909,7 +6026,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>192</v>
       </c>
@@ -5935,7 +6052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>194</v>
       </c>
@@ -5964,7 +6081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>195</v>
       </c>
@@ -5990,7 +6107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>196</v>
       </c>
@@ -6016,7 +6133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>197</v>
       </c>
@@ -6042,7 +6159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>198</v>
       </c>
@@ -6068,7 +6185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>199</v>
       </c>
@@ -6091,6 +6208,957 @@
         <v>-1</v>
       </c>
       <c r="I187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>200</v>
+      </c>
+      <c r="B188">
+        <v>36</v>
+      </c>
+      <c r="C188" t="s">
+        <v>12</v>
+      </c>
+      <c r="D188">
+        <v>14</v>
+      </c>
+      <c r="F188">
+        <v>66000</v>
+      </c>
+      <c r="G188">
+        <v>0</v>
+      </c>
+      <c r="H188">
+        <v>-1</v>
+      </c>
+      <c r="I188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>201</v>
+      </c>
+      <c r="B189">
+        <v>20</v>
+      </c>
+      <c r="C189" t="s">
+        <v>12</v>
+      </c>
+      <c r="D189">
+        <v>30</v>
+      </c>
+      <c r="F189">
+        <v>0</v>
+      </c>
+      <c r="G189">
+        <v>0</v>
+      </c>
+      <c r="H189">
+        <v>-1</v>
+      </c>
+      <c r="I189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>202</v>
+      </c>
+      <c r="B190">
+        <v>26</v>
+      </c>
+      <c r="C190" t="s">
+        <v>12</v>
+      </c>
+      <c r="D190">
+        <v>14</v>
+      </c>
+      <c r="F190">
+        <v>38000</v>
+      </c>
+      <c r="G190">
+        <v>0</v>
+      </c>
+      <c r="H190">
+        <v>-1</v>
+      </c>
+      <c r="I190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>203</v>
+      </c>
+      <c r="B191">
+        <v>28</v>
+      </c>
+      <c r="C191" t="s">
+        <v>12</v>
+      </c>
+      <c r="D191">
+        <v>11</v>
+      </c>
+      <c r="F191">
+        <v>-1</v>
+      </c>
+      <c r="G191">
+        <v>0</v>
+      </c>
+      <c r="H191">
+        <v>-1</v>
+      </c>
+      <c r="I191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>204</v>
+      </c>
+      <c r="B192">
+        <v>37</v>
+      </c>
+      <c r="C192" t="s">
+        <v>6</v>
+      </c>
+      <c r="D192">
+        <v>5</v>
+      </c>
+      <c r="F192">
+        <v>67000</v>
+      </c>
+      <c r="G192">
+        <v>0</v>
+      </c>
+      <c r="H192">
+        <v>800</v>
+      </c>
+      <c r="I192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>205</v>
+      </c>
+      <c r="B193">
+        <v>27</v>
+      </c>
+      <c r="C193" t="s">
+        <v>6</v>
+      </c>
+      <c r="D193">
+        <v>5</v>
+      </c>
+      <c r="F193">
+        <v>46500</v>
+      </c>
+      <c r="G193">
+        <v>0</v>
+      </c>
+      <c r="H193">
+        <v>-1</v>
+      </c>
+      <c r="I193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>206</v>
+      </c>
+      <c r="B194">
+        <v>28</v>
+      </c>
+      <c r="C194" t="s">
+        <v>6</v>
+      </c>
+      <c r="D194">
+        <v>11</v>
+      </c>
+      <c r="F194">
+        <v>57000</v>
+      </c>
+      <c r="G194">
+        <v>0</v>
+      </c>
+      <c r="H194">
+        <v>-1</v>
+      </c>
+      <c r="I194">
+        <v>1</v>
+      </c>
+      <c r="J194" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>207</v>
+      </c>
+      <c r="B195">
+        <v>24</v>
+      </c>
+      <c r="C195" t="s">
+        <v>6</v>
+      </c>
+      <c r="D195">
+        <v>3</v>
+      </c>
+      <c r="F195">
+        <v>0</v>
+      </c>
+      <c r="G195">
+        <v>-100</v>
+      </c>
+      <c r="H195">
+        <v>-1</v>
+      </c>
+      <c r="I195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>208</v>
+      </c>
+      <c r="B196">
+        <v>33</v>
+      </c>
+      <c r="C196" t="s">
+        <v>12</v>
+      </c>
+      <c r="D196">
+        <v>30</v>
+      </c>
+      <c r="F196">
+        <v>71500</v>
+      </c>
+      <c r="G196">
+        <v>-150</v>
+      </c>
+      <c r="H196">
+        <v>1200</v>
+      </c>
+      <c r="I196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>209</v>
+      </c>
+      <c r="B197">
+        <v>28</v>
+      </c>
+      <c r="C197" t="s">
+        <v>6</v>
+      </c>
+      <c r="D197">
+        <v>2</v>
+      </c>
+      <c r="F197">
+        <v>52000</v>
+      </c>
+      <c r="G197">
+        <v>0</v>
+      </c>
+      <c r="H197">
+        <v>-1</v>
+      </c>
+      <c r="I197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>210</v>
+      </c>
+      <c r="B198">
+        <v>27</v>
+      </c>
+      <c r="C198" t="s">
+        <v>6</v>
+      </c>
+      <c r="D198">
+        <v>3</v>
+      </c>
+      <c r="F198">
+        <v>48000</v>
+      </c>
+      <c r="G198">
+        <v>0</v>
+      </c>
+      <c r="H198">
+        <v>-1</v>
+      </c>
+      <c r="I198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>211</v>
+      </c>
+      <c r="B199">
+        <v>24</v>
+      </c>
+      <c r="C199" t="s">
+        <v>6</v>
+      </c>
+      <c r="D199">
+        <v>4</v>
+      </c>
+      <c r="F199">
+        <v>0</v>
+      </c>
+      <c r="G199">
+        <v>0</v>
+      </c>
+      <c r="H199">
+        <v>-1</v>
+      </c>
+      <c r="I199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>212</v>
+      </c>
+      <c r="B200">
+        <v>25</v>
+      </c>
+      <c r="C200" t="s">
+        <v>12</v>
+      </c>
+      <c r="D200">
+        <v>5</v>
+      </c>
+      <c r="F200">
+        <v>37000</v>
+      </c>
+      <c r="G200">
+        <v>0</v>
+      </c>
+      <c r="H200">
+        <v>-1</v>
+      </c>
+      <c r="I200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>213</v>
+      </c>
+      <c r="B201">
+        <v>27</v>
+      </c>
+      <c r="C201" t="s">
+        <v>12</v>
+      </c>
+      <c r="D201">
+        <v>12</v>
+      </c>
+      <c r="F201">
+        <v>51000</v>
+      </c>
+      <c r="G201">
+        <v>0</v>
+      </c>
+      <c r="H201">
+        <v>-1</v>
+      </c>
+      <c r="I201">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>214</v>
+      </c>
+      <c r="B202">
+        <v>32</v>
+      </c>
+      <c r="C202" t="s">
+        <v>12</v>
+      </c>
+      <c r="D202">
+        <v>14</v>
+      </c>
+      <c r="F202">
+        <v>62000</v>
+      </c>
+      <c r="G202">
+        <v>0</v>
+      </c>
+      <c r="H202">
+        <v>-1</v>
+      </c>
+      <c r="I202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>215</v>
+      </c>
+      <c r="B203">
+        <v>38</v>
+      </c>
+      <c r="C203" t="s">
+        <v>12</v>
+      </c>
+      <c r="D203">
+        <v>1</v>
+      </c>
+      <c r="F203">
+        <v>87000</v>
+      </c>
+      <c r="G203">
+        <v>0</v>
+      </c>
+      <c r="H203">
+        <v>2000</v>
+      </c>
+      <c r="I203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>216</v>
+      </c>
+      <c r="B204">
+        <v>38</v>
+      </c>
+      <c r="C204" t="s">
+        <v>6</v>
+      </c>
+      <c r="D204">
+        <v>2</v>
+      </c>
+      <c r="F204">
+        <v>93000</v>
+      </c>
+      <c r="G204">
+        <v>0</v>
+      </c>
+      <c r="H204">
+        <v>2100</v>
+      </c>
+      <c r="I204">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>217</v>
+      </c>
+      <c r="B205">
+        <v>37</v>
+      </c>
+      <c r="C205" t="s">
+        <v>6</v>
+      </c>
+      <c r="D205">
+        <v>4</v>
+      </c>
+      <c r="E205">
+        <v>1</v>
+      </c>
+      <c r="F205">
+        <v>87000</v>
+      </c>
+      <c r="G205">
+        <v>-650</v>
+      </c>
+      <c r="H205">
+        <v>1800</v>
+      </c>
+      <c r="I205">
+        <v>1</v>
+      </c>
+      <c r="K205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>218</v>
+      </c>
+      <c r="B206">
+        <v>28</v>
+      </c>
+      <c r="C206" t="s">
+        <v>6</v>
+      </c>
+      <c r="D206">
+        <v>20</v>
+      </c>
+      <c r="F206">
+        <v>0</v>
+      </c>
+      <c r="G206">
+        <v>300</v>
+      </c>
+      <c r="H206">
+        <v>-1</v>
+      </c>
+      <c r="I206">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>219</v>
+      </c>
+      <c r="B207">
+        <v>25</v>
+      </c>
+      <c r="C207" t="s">
+        <v>6</v>
+      </c>
+      <c r="D207">
+        <v>20</v>
+      </c>
+      <c r="F207">
+        <v>56000</v>
+      </c>
+      <c r="G207">
+        <v>0</v>
+      </c>
+      <c r="H207">
+        <v>-1</v>
+      </c>
+      <c r="I207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>220</v>
+      </c>
+      <c r="B208">
+        <v>26</v>
+      </c>
+      <c r="C208" t="s">
+        <v>12</v>
+      </c>
+      <c r="D208">
+        <v>20</v>
+      </c>
+      <c r="F208">
+        <v>28500</v>
+      </c>
+      <c r="G208">
+        <v>0</v>
+      </c>
+      <c r="H208">
+        <v>-1</v>
+      </c>
+      <c r="I208">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>221</v>
+      </c>
+      <c r="B209">
+        <v>27</v>
+      </c>
+      <c r="C209" t="s">
+        <v>6</v>
+      </c>
+      <c r="D209">
+        <v>13</v>
+      </c>
+      <c r="F209">
+        <v>41000</v>
+      </c>
+      <c r="G209">
+        <v>0</v>
+      </c>
+      <c r="H209">
+        <v>-1</v>
+      </c>
+      <c r="I209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>222</v>
+      </c>
+      <c r="B210">
+        <v>29</v>
+      </c>
+      <c r="C210" t="s">
+        <v>6</v>
+      </c>
+      <c r="D210">
+        <v>21</v>
+      </c>
+      <c r="F210">
+        <v>74500</v>
+      </c>
+      <c r="G210">
+        <v>-1000</v>
+      </c>
+      <c r="H210">
+        <v>1400</v>
+      </c>
+      <c r="I210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>223</v>
+      </c>
+      <c r="B211">
+        <v>33</v>
+      </c>
+      <c r="C211" t="s">
+        <v>6</v>
+      </c>
+      <c r="D211">
+        <v>13</v>
+      </c>
+      <c r="F211">
+        <v>67000</v>
+      </c>
+      <c r="G211">
+        <v>-500</v>
+      </c>
+      <c r="H211">
+        <v>900</v>
+      </c>
+      <c r="I211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>224</v>
+      </c>
+      <c r="B212">
+        <v>34</v>
+      </c>
+      <c r="C212" t="s">
+        <v>6</v>
+      </c>
+      <c r="D212">
+        <v>20</v>
+      </c>
+      <c r="F212">
+        <v>63500</v>
+      </c>
+      <c r="G212">
+        <v>-400</v>
+      </c>
+      <c r="H212">
+        <v>850</v>
+      </c>
+      <c r="I212">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>225</v>
+      </c>
+      <c r="B213">
+        <v>36</v>
+      </c>
+      <c r="C213" t="s">
+        <v>6</v>
+      </c>
+      <c r="D213">
+        <v>1</v>
+      </c>
+      <c r="F213">
+        <v>79500</v>
+      </c>
+      <c r="G213">
+        <v>-200</v>
+      </c>
+      <c r="H213">
+        <v>1200</v>
+      </c>
+      <c r="I213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>226</v>
+      </c>
+      <c r="B214">
+        <v>37</v>
+      </c>
+      <c r="C214" t="s">
+        <v>6</v>
+      </c>
+      <c r="D214">
+        <v>1</v>
+      </c>
+      <c r="F214">
+        <v>77000</v>
+      </c>
+      <c r="G214">
+        <v>-350</v>
+      </c>
+      <c r="H214">
+        <v>1300</v>
+      </c>
+      <c r="I214">
+        <v>0</v>
+      </c>
+      <c r="J214" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>227</v>
+      </c>
+      <c r="B215">
+        <v>31</v>
+      </c>
+      <c r="C215" t="s">
+        <v>6</v>
+      </c>
+      <c r="D215">
+        <v>4</v>
+      </c>
+      <c r="F215">
+        <v>67000</v>
+      </c>
+      <c r="G215">
+        <v>0</v>
+      </c>
+      <c r="H215">
+        <v>800</v>
+      </c>
+      <c r="I215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>228</v>
+      </c>
+      <c r="B216">
+        <v>33</v>
+      </c>
+      <c r="C216" t="s">
+        <v>6</v>
+      </c>
+      <c r="D216">
+        <v>3</v>
+      </c>
+      <c r="F216">
+        <v>59000</v>
+      </c>
+      <c r="G216">
+        <v>-200</v>
+      </c>
+      <c r="H216">
+        <v>-1</v>
+      </c>
+      <c r="I216">
+        <v>1</v>
+      </c>
+      <c r="K216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>229</v>
+      </c>
+      <c r="B217">
+        <v>28</v>
+      </c>
+      <c r="C217" t="s">
+        <v>6</v>
+      </c>
+      <c r="D217">
+        <v>5</v>
+      </c>
+      <c r="F217">
+        <v>65000</v>
+      </c>
+      <c r="G217">
+        <v>-100</v>
+      </c>
+      <c r="H217">
+        <v>-1</v>
+      </c>
+      <c r="I217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>230</v>
+      </c>
+      <c r="B218">
+        <v>31</v>
+      </c>
+      <c r="C218" t="s">
+        <v>12</v>
+      </c>
+      <c r="D218">
+        <v>2</v>
+      </c>
+      <c r="F218">
+        <v>64500</v>
+      </c>
+      <c r="G218">
+        <v>100</v>
+      </c>
+      <c r="H218">
+        <v>-1</v>
+      </c>
+      <c r="I218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>231</v>
+      </c>
+      <c r="B219">
+        <v>28</v>
+      </c>
+      <c r="C219" t="s">
+        <v>6</v>
+      </c>
+      <c r="D219">
+        <v>1</v>
+      </c>
+      <c r="F219">
+        <v>57500</v>
+      </c>
+      <c r="G219">
+        <v>0</v>
+      </c>
+      <c r="H219">
+        <v>-1</v>
+      </c>
+      <c r="I219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>232</v>
+      </c>
+      <c r="B220">
+        <v>29</v>
+      </c>
+      <c r="C220" t="s">
+        <v>12</v>
+      </c>
+      <c r="D220">
+        <v>20</v>
+      </c>
+      <c r="F220">
+        <v>9999999</v>
+      </c>
+      <c r="G220">
+        <v>0</v>
+      </c>
+      <c r="H220">
+        <v>-1</v>
+      </c>
+      <c r="I220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>233</v>
+      </c>
+      <c r="B221">
+        <v>28</v>
+      </c>
+      <c r="C221" t="s">
+        <v>12</v>
+      </c>
+      <c r="D221">
+        <v>30</v>
+      </c>
+      <c r="F221">
+        <v>73000</v>
+      </c>
+      <c r="G221">
+        <v>0</v>
+      </c>
+      <c r="H221">
+        <v>-1</v>
+      </c>
+      <c r="I221">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>234</v>
+      </c>
+      <c r="B222">
+        <v>27</v>
+      </c>
+      <c r="C222" t="s">
+        <v>12</v>
+      </c>
+      <c r="D222">
+        <v>30</v>
+      </c>
+      <c r="F222">
+        <v>71000</v>
+      </c>
+      <c r="G222">
+        <v>0</v>
+      </c>
+      <c r="H222">
+        <v>-1</v>
+      </c>
+      <c r="I222">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>235</v>
+      </c>
+      <c r="B223">
+        <v>31</v>
+      </c>
+      <c r="C223" t="s">
+        <v>6</v>
+      </c>
+      <c r="D223">
+        <v>20</v>
+      </c>
+      <c r="F223">
+        <v>68500</v>
+      </c>
+      <c r="G223">
+        <v>0</v>
+      </c>
+      <c r="H223">
+        <v>-1</v>
+      </c>
+      <c r="I223">
         <v>1</v>
       </c>
     </row>
@@ -6100,14 +7168,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="503cb35d-549b-4020-be52-0b9d6cf7fa62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FC116FBE851056418397D23CE15C02B5" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d6247c4b58aafea520bb9699c52d3d0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1105192a-0549-48ad-943a-7717d3fc4905" xmlns:ns4="503cb35d-549b-4020-be52-0b9d6cf7fa62" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="130a2f1d92904d3f1a1fa4025249897e" ns3:_="" ns4:_="">
     <xsd:import namespace="1105192a-0549-48ad-943a-7717d3fc4905"/>
@@ -6332,6 +7392,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="503cb35d-549b-4020-be52-0b9d6cf7fa62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6342,16 +7410,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53A9EB78-4379-476A-BE51-361A2C7F77F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="503cb35d-549b-4020-be52-0b9d6cf7fa62"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD6594CA-5E76-4D5F-8479-3669252C60F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6370,6 +7428,16 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53A9EB78-4379-476A-BE51-361A2C7F77F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="503cb35d-549b-4020-be52-0b9d6cf7fa62"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DFE2C9F-45A3-4E9C-83C1-2B347328CE0A}">
   <ds:schemaRefs>

</xml_diff>